<commit_message>
v2.0.1 - commit after migrated to xCode 12.3
</commit_message>
<xml_diff>
--- a/PowerPoints/Calculations.xlsx
+++ b/PowerPoints/Calculations.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hardygermany/CoBaT/CoBaT/PowerPoints/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{526654F1-524C-004C-946F-4C0CA9DF553D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F4472EB-4841-8349-ADED-2D076DB85242}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16900" xr2:uid="{3C0AA6CE-39B1-E347-AF02-1CD34B4C02A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -68,7 +68,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -101,7 +101,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -420,7 +420,7 @@
   <dimension ref="B2:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:J16"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -482,7 +482,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="1">
-        <f t="shared" ref="F6:I13" si="0">$D6*F$3</f>
+        <f t="shared" ref="F6:I10" si="0">$D6*F$3</f>
         <v>0.53333333333333333</v>
       </c>
       <c r="G6" s="1">
@@ -600,7 +600,7 @@
         <v>2</v>
       </c>
       <c r="J11" s="1">
-        <f t="shared" ref="J11:J13" si="1">ROUND(I11,0)</f>
+        <f t="shared" ref="J11:J12" si="1">ROUND(I11,0)</f>
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V2.2.0.4 - added overlays and first attempt to annotations
</commit_message>
<xml_diff>
--- a/PowerPoints/Calculations.xlsx
+++ b/PowerPoints/Calculations.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hardygermany/CoBaT/CoBaT/PowerPoints/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F4472EB-4841-8349-ADED-2D076DB85242}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCBBD894-E7BA-C54E-B500-2F4207C57BD7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16900" xr2:uid="{3C0AA6CE-39B1-E347-AF02-1CD34B4C02A7}"/>
+    <workbookView xWindow="7360" yWindow="500" windowWidth="21060" windowHeight="16720" activeTab="1" xr2:uid="{3C0AA6CE-39B1-E347-AF02-1CD34B4C02A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Balkenbreite</t>
   </si>
@@ -61,16 +62,37 @@
   </si>
   <si>
     <t>Summe Balken</t>
+  </si>
+  <si>
+    <t>MKMapRect.origin.x</t>
+  </si>
+  <si>
+    <t>MKMapRect.origin.y</t>
+  </si>
+  <si>
+    <t>MKMapRect.size.width</t>
+  </si>
+  <si>
+    <t>MKMapRect.size.height</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="170" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -96,15 +118,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Komma" xfId="1" builtinId="3"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -419,7 +444,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2630461-86B7-FD4D-8A22-B4B9162E4A35}">
   <dimension ref="B2:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
@@ -682,4 +707,128 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1A5817B-F6E5-D14B-A67B-04ECB823B798}">
+  <dimension ref="A6:C33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B6" s="3"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="3">
+        <v>139734336</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="3">
+        <v>90533184</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="3">
+        <v>25984</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="3">
+        <v>25984</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B11" s="3"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B12" s="3"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B13" s="3"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B14" s="3"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B15" s="3"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B16" s="3"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B18" s="3"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B19" s="3"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B20" s="3"/>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B21" s="3"/>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B22" s="3"/>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B23" s="3"/>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B24" s="3"/>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B25" s="3"/>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B26" s="3"/>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B28" s="3"/>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B29" s="3"/>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B30" s="3"/>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B31" s="3"/>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B32" s="3"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B33" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>